<commit_message>
feat: add truth label for instructions in this proj
</commit_message>
<xml_diff>
--- a/ketang/sp21/sp21-proj3-starter/Book1.xlsx
+++ b/ketang/sp21/sp21-proj3-starter/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ketang/MyCS61C/ketang/sp21/sp21-proj3-starter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D45F16C0-FCEA-CD4F-8F75-B7E879243A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7BD3F0-99F2-9849-BBCF-29570CDE312A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="5640" windowWidth="28040" windowHeight="17440" xr2:uid="{8EE1AFFD-A597-2F44-A2B0-7A9A818A6048}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" xr2:uid="{8EE1AFFD-A597-2F44-A2B0-7A9A818A6048}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>inst</t>
   </si>
@@ -155,37 +155,61 @@
     <t>csrwi</t>
   </si>
   <si>
-    <t>breq</t>
-  </si>
-  <si>
-    <t>brlt</t>
-  </si>
-  <si>
-    <t>pcsel</t>
-  </si>
-  <si>
-    <t>immsel</t>
-  </si>
-  <si>
-    <t>brun</t>
-  </si>
-  <si>
-    <t>asel</t>
-  </si>
-  <si>
-    <t>bsel</t>
-  </si>
-  <si>
-    <t>alusel</t>
-  </si>
-  <si>
-    <t>memrw</t>
-  </si>
-  <si>
-    <t>regwen</t>
-  </si>
-  <si>
-    <t>wbsel</t>
+    <t>BrEq</t>
+  </si>
+  <si>
+    <t>BrLt</t>
+  </si>
+  <si>
+    <t>ImmSel</t>
+  </si>
+  <si>
+    <t>BrUn</t>
+  </si>
+  <si>
+    <t>Asel(1:选rs1,0:选pc)</t>
+  </si>
+  <si>
+    <t>Bsel(1:选rs2, 0:选imm)</t>
+  </si>
+  <si>
+    <t>MemRW(0:read,1:write)</t>
+  </si>
+  <si>
+    <t>RegWEn(0:不写回reg，1:写回reg)</t>
+  </si>
+  <si>
+    <t>WBSel(0:data from mem,1:aluresult,2:pc+4)</t>
+  </si>
+  <si>
+    <t>ALUSel(decimal值，看alu.circ的表)</t>
+  </si>
+  <si>
+    <t>PCSel(0:pc+4, 1:aluresult)</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>0(因为无符号的blt是bltu指令，所以认为这里是比较有符号，所以写0)</t>
+  </si>
+  <si>
+    <t>UJ</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -201,17 +225,125 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -221,13 +353,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -537,243 +694,1077 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB45812B-1177-8547-B4F4-A106F379297B}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>13</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+      <c r="I35" s="10">
+        <v>15</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0</v>
+      </c>
+      <c r="K35" s="11">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1</v>
+      </c>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D36" s="12">
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1</v>
+      </c>
+      <c r="L36" s="12">
+        <v>2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D37" s="12">
+        <v>1</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1</v>
+      </c>
+      <c r="H37" s="12">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <v>0</v>
+      </c>
+      <c r="J37" s="12">
+        <v>0</v>
+      </c>
+      <c r="K37" s="12">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="M2:M13"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="M14:M24"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="M34:M35"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2:L39">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>